<commit_message>
add case home page
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -7,10 +7,9 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="1" sheetId="1" r:id="rId1"/>
     <sheet name="HomePage" sheetId="2" r:id="rId2"/>
     <sheet name="SignIn" sheetId="3" r:id="rId3"/>
-    <sheet name="test" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -22,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="100">
   <si>
     <t>tld01@mailinator.com</t>
   </si>
@@ -226,6 +225,102 @@
   </si>
   <si>
     <t>ptnquynhta@gmail.com</t>
+  </si>
+  <si>
+    <t>Cổng thông tin đào tạo</t>
+  </si>
+  <si>
+    <t>Các ngành đào tạo</t>
+  </si>
+  <si>
+    <t>Chức năng nhiệm vụ</t>
+  </si>
+  <si>
+    <t>Quy chế - quy định</t>
+  </si>
+  <si>
+    <t>nB_GT</t>
+  </si>
+  <si>
+    <t>Thông báo chung</t>
+  </si>
+  <si>
+    <t>Thông báo từ Công tác sinh viên</t>
+  </si>
+  <si>
+    <t>Thông báo từ Phòng Kế hoạch tài chính</t>
+  </si>
+  <si>
+    <t>nB_TB</t>
+  </si>
+  <si>
+    <t>Lịch thi</t>
+  </si>
+  <si>
+    <t>Lịch GVCN họp lớp định kỳ</t>
+  </si>
+  <si>
+    <t>Biểu đồ giảng dạy</t>
+  </si>
+  <si>
+    <t>Danh sách lớp sinh hoạt K21</t>
+  </si>
+  <si>
+    <t>nB_TKB</t>
+  </si>
+  <si>
+    <t>Biểu mẫu sinh viên</t>
+  </si>
+  <si>
+    <t>Quy trình giảng viên</t>
+  </si>
+  <si>
+    <t>Quy trình sinh viên</t>
+  </si>
+  <si>
+    <t>nB_QT</t>
+  </si>
+  <si>
+    <t>Kế hoạch năm</t>
+  </si>
+  <si>
+    <t>Chương trình kỹ sư/cử nhân toàn cầu</t>
+  </si>
+  <si>
+    <t>Đề án mở ngành mới</t>
+  </si>
+  <si>
+    <t>nB_L</t>
+  </si>
+  <si>
+    <t>Lịch thời khóa biểu</t>
+  </si>
+  <si>
+    <t>Lịch sinh hoạt lớp chủ nhiệm</t>
+  </si>
+  <si>
+    <t>Lịch seminar cấp Khoa</t>
+  </si>
+  <si>
+    <t>Lịch phòng học</t>
+  </si>
+  <si>
+    <t>nB_CTĐT</t>
+  </si>
+  <si>
+    <t>Sinh viên</t>
+  </si>
+  <si>
+    <t>Giảng viên</t>
+  </si>
+  <si>
+    <t>Bộ phận khác</t>
+  </si>
+  <si>
+    <t>Phụ huynh</t>
+  </si>
+  <si>
+    <t>nB_K</t>
   </si>
 </sst>
 </file>
@@ -254,15 +349,21 @@
       <name val="Inherit"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -294,18 +395,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -327,6 +435,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -611,7 +722,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -650,171 +761,283 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:N9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="39.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="36.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="16.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="36.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.28515625" style="9" customWidth="1"/>
+    <col min="9" max="9" width="35.140625" style="9" customWidth="1"/>
+    <col min="10" max="10" width="26.28515625" style="9" customWidth="1"/>
+    <col min="11" max="11" width="19.7109375" style="9" customWidth="1"/>
+    <col min="12" max="12" width="33.85546875" style="9" customWidth="1"/>
+    <col min="13" max="13" width="27.7109375" style="9" customWidth="1"/>
+    <col min="14" max="14" width="19.28515625" style="9" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" ht="16.5" customHeight="1">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:14" s="11" customFormat="1" ht="16.5" customHeight="1">
+      <c r="A1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="11" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="2" t="s">
+      <c r="H1" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="K1" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="L1" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="M1" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="N1" s="11" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="9" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="2" t="s">
+      <c r="H2" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="K2" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="L2" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="M2" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="N2" s="9" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="9" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="2" t="s">
+      <c r="H3" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="J3" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="K3" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="L3" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="M3" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="N3" s="9" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="9" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="2" t="s">
+      <c r="H4" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="J4" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="K4" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="L4" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="M4" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="N4" s="9" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" s="9" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="2" t="s">
+      <c r="H5" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="J5" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="L5" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="M5" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="N5" s="9" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="9" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="2" t="s">
+      <c r="J6" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="M6" s="9" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G7" s="9" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="2" t="s">
+    <row r="8" spans="1:14">
+      <c r="A8" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="G8" s="9" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
-      <c r="E9" s="2" t="s">
+    <row r="9" spans="1:14">
+      <c r="E9" s="9" t="s">
         <v>33</v>
       </c>
     </row>
@@ -828,230 +1051,230 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="5.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.5703125" style="6" customWidth="1"/>
-    <col min="4" max="4" width="19.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="58.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="6"/>
+    <col min="1" max="1" width="5.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="58.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="3" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="6">
+      <c r="A2" s="2">
         <v>4</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="2">
         <v>123</v>
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="6">
+      <c r="A4" s="2">
         <v>7</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="2" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="6">
+      <c r="A5" s="2">
         <v>8</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="2" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="6">
+      <c r="A6" s="2">
         <v>9</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="2" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="6">
+      <c r="A7" s="2">
         <v>10</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="2" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="6">
+      <c r="A8" s="2">
         <v>11</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="2" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="6">
+      <c r="A9" s="2">
         <v>12</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="2" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="6">
+      <c r="A10" s="2">
         <v>13</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="2" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="6">
+      <c r="A11" s="2">
         <v>14</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E11" s="2" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="6">
+      <c r="A12" s="2">
         <v>15</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="E12" s="2" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="6">
+      <c r="A13" s="2">
         <v>16</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="E13" s="2" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="6">
+      <c r="A14" s="2">
         <v>17</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="E14" s="6" t="s">
+      <c r="E14" s="2" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="30">
-      <c r="A15" s="6">
+      <c r="A15" s="2">
         <v>18</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="E15" s="2" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="30">
-      <c r="A16" s="6">
+      <c r="A16" s="2">
         <v>19</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="E16" s="6" t="s">
+      <c r="E16" s="2" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="30">
-      <c r="A17" s="6">
+      <c r="A17" s="2">
         <v>20</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C17" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="E17" s="6" t="s">
+      <c r="E17" s="2" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="6">
+      <c r="A18" s="2">
         <v>21</v>
       </c>
-      <c r="B18" s="12" t="s">
+      <c r="B18" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="C18" s="10" t="s">
+      <c r="C18" s="6" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1068,16 +1291,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId8"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
fix integrate test HomePage
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -9,7 +9,8 @@
   <sheets>
     <sheet name="1" sheetId="1" r:id="rId1"/>
     <sheet name="HomePage" sheetId="2" r:id="rId2"/>
-    <sheet name="SignIn" sheetId="3" r:id="rId3"/>
+    <sheet name="HP" sheetId="4" r:id="rId3"/>
+    <sheet name="SignIn" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="125">
   <si>
     <t>tld01@mailinator.com</t>
   </si>
@@ -321,6 +322,81 @@
   </si>
   <si>
     <t>nB_K</t>
+  </si>
+  <si>
+    <t>field</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>Tin tức sự kiện,Thông báo,Danh bạ,Biểu mẫu,Lịch tuần,Hình ảnh,Email</t>
+  </si>
+  <si>
+    <t>topBar_rightMenu</t>
+  </si>
+  <si>
+    <t>Đoàn thể,Trung tâm,Phòng,Khoa</t>
+  </si>
+  <si>
+    <t>Đảng bộ,Công Đoàn,* Đoàn Thanh niên</t>
+  </si>
+  <si>
+    <t>* Trung tâm học liệu &amp; Truyền thông,* Trung tâm Ngoại ngữ Tin học,* Trung tâm Quản trị và phát triển CNTT,* Tổ Quản lý Ký túc xá &amp; Phục vụ cộng đồng</t>
+  </si>
+  <si>
+    <t>* Phòng Tổ chức - Hành chính,* Phòng Đào tạo,* Phòng Công tác sinh viên,* Phòng Quản lý Khoa học &amp; HTQT,* Phòng Khảo thí &amp; ĐBCLGD,* Phòng Thanh tra - Pháp chế,* Phòng Cơ sở vật chất,* Phòng Kế hoạch - Tài chính</t>
+  </si>
+  <si>
+    <t>* Khoa Khoa học máy tính,* Khoa Kỹ thuật máy tính và Điện tử,* Khoa Kinh tế số &amp; thương mại điện tử,* Tổ cơ bản</t>
+  </si>
+  <si>
+    <t>navBar</t>
+  </si>
+  <si>
+    <t>Giới thiệu,Thông báo,Thời khoá biểu,Quy trình,Chương trình đào tạo,Lịch,Đăng nhập</t>
+  </si>
+  <si>
+    <t>navBar_TB</t>
+  </si>
+  <si>
+    <t>navBar_TKB</t>
+  </si>
+  <si>
+    <t>navBar_QT</t>
+  </si>
+  <si>
+    <t>navBar_L</t>
+  </si>
+  <si>
+    <t>navBar_K</t>
+  </si>
+  <si>
+    <t>navBar_GT</t>
+  </si>
+  <si>
+    <t>Cổng thông tin đào tạo,Các ngành đào tạo,Chức năng nhiệm vụ,Quy chế - quy định</t>
+  </si>
+  <si>
+    <t>Thông báo chung,Thông báo từ Công tác sinh viên,Thông báo từ Phòng Kế hoạch tài chính</t>
+  </si>
+  <si>
+    <t>Thời khoá biểu,Lịch thi,Lịch GVCN họp lớp định kỳ,Biểu đồ giảng dạy,Danh sách lớp sinh hoạt K21</t>
+  </si>
+  <si>
+    <t>Biểu mẫu sinh viên,Quy trình giảng viên,Quy trình sinh viên</t>
+  </si>
+  <si>
+    <t>Kế hoạch năm,Chương trình đào tạo,Chương trình kỹ sư/cử nhân toàn cầu,Đề án mở ngành mới</t>
+  </si>
+  <si>
+    <t>Lịch thời khóa biểu,Lịch sinh hoạt lớp chủ nhiệm,Lịch seminar cấp Khoa,Lịch thi,Lịch phòng học</t>
+  </si>
+  <si>
+    <t>Sinh viên,Giảng viên,Bộ phận khác,Phụ huynh</t>
+  </si>
+  <si>
+    <t>navBar_CTDT</t>
   </si>
 </sst>
 </file>
@@ -363,7 +439,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -406,12 +482,25 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -438,6 +527,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -764,7 +868,7 @@
   <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1049,9 +1153,149 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="17.5703125" style="12" customWidth="1"/>
+    <col min="2" max="2" width="152.85546875" style="13" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="13"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="12" customFormat="1">
+      <c r="A1" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="30">
+      <c r="A6" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>123</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>

</xml_diff>